<commit_message>
maruta BECCS 5 net-zero
</commit_message>
<xml_diff>
--- a/xlsx/sample.xlsx
+++ b/xlsx/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\TA\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6B6277-93E0-4A82-8F81-53213F6B414A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD175D2-40A4-46B0-8980-FA0CBFB8D338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{C4CD650B-609C-4368-B8A9-F4143D92654C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{C4CD650B-609C-4368-B8A9-F4143D92654C}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP・人口・省エネ" sheetId="1" r:id="rId1"/>
@@ -436,10 +436,10 @@
                   <c:v>0.98472804099484257</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47304163446537506</c:v>
+                  <c:v>0.44521565596741242</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5118602122381706E-14</c:v>
+                  <c:v>1.2532525443553324E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,10 +507,10 @@
                   <c:v>1.4615669781087863</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99366267885242066</c:v>
+                  <c:v>0.69354872739083917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53724266391901232</c:v>
+                  <c:v>8.9069178491848464E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,10 +578,10 @@
                   <c:v>2.1290218835980919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4467271034407692</c:v>
+                  <c:v>1.1230320398839735</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.74365310327521483</c:v>
+                  <c:v>0.23242347346729614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -649,10 +649,10 @@
                   <c:v>0.22490521403835756</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64349706953537633</c:v>
+                  <c:v>0.81886298748032282</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95855016884281175</c:v>
+                  <c:v>1.124328332989021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,10 +720,10 @@
                   <c:v>0.83659218770554256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8154057483588999</c:v>
+                  <c:v>1.975655163068359</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5533049081770285</c:v>
+                  <c:v>2.5271172148608767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1071,10 +1071,10 @@
                   <c:v>101.81273444054483</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.662321331106526</c:v>
+                  <c:v>47.800982076925457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.582582187331333</c:v>
+                  <c:v>6.8939544152688841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1386,10 +1386,10 @@
                   <c:v>41.590868044025868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.795342362285162</c:v>
+                  <c:v>20.006125894552333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4993407873359121</c:v>
+                  <c:v>3.5227530894879102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,13 +1698,13 @@
                   <c:v>449.00553720294573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94.40609546285782</c:v>
+                  <c:v>94.406095462858929</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.31232648279615</c:v>
+                  <c:v>103.29708990367854</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.861109719592633</c:v>
+                  <c:v>-20.914565787064184</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2075,13 +2075,13 @@
                   <c:v>906.13930847649056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>420.12477991644295</c:v>
+                  <c:v>420.12477991644403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>320.13294694942516</c:v>
+                  <c:v>262.09725989573758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.16263100066517</c:v>
+                  <c:v>-0.98165451027861295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2442,10 +2442,10 @@
                   <c:v>0.14263481989429305</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4191788999916052E-2</c:v>
+                  <c:v>6.0415801411685767E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9086693609402903E-15</c:v>
+                  <c:v>1.5821864439373547E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2513,10 +2513,10 @@
                   <c:v>1.1410785591543242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83449325699889487</c:v>
+                  <c:v>0.54374221270516765</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5372426639190071</c:v>
+                  <c:v>8.9069178491844106E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2655,10 +2655,10 @@
                   <c:v>-3.1671292231980848E-16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1283835779998321</c:v>
+                  <c:v>0.24166320564674307</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.21489706556760357</c:v>
+                  <c:v>0.35627671396734478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2726,10 +2726,10 @@
                   <c:v>0.14263481989429053</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2567671559996596</c:v>
+                  <c:v>0.36249480847010601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32234559835140347</c:v>
+                  <c:v>0.44534589245917622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3033,10 +3033,10 @@
                   <c:v>0.2011163831916164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0511001758407539E-2</c:v>
+                  <c:v>8.5186825184383669E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6912410228122979E-15</c:v>
+                  <c:v>2.2308971636470485E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3175,10 +3175,10 @@
                   <c:v>0.40223276638322564</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2715330052752194</c:v>
+                  <c:v>0.21296706296095616</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15150340084377287</c:v>
+                  <c:v>6.2794172718140806E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3246,10 +3246,10 @@
                   <c:v>0.1005581915958082</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1357665026376097</c:v>
+                  <c:v>0.12778023777657399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15150340084377018</c:v>
+                  <c:v>0.12558834543628386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3317,10 +3317,10 @@
                   <c:v>0.30167457478741744</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40729950791282749</c:v>
+                  <c:v>0.42593412592191232</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45451020253131325</c:v>
+                  <c:v>0.43955920902699236</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3624,10 +3624,10 @@
                   <c:v>0.2486940448851038</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12201629038177052</c:v>
+                  <c:v>0.11483886153578417</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0212986167245552E-15</c:v>
+                  <c:v>3.3334449059690571E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3695,10 +3695,10 @@
                   <c:v>0.1243470224425519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1008145190885259E-2</c:v>
+                  <c:v>5.7419430767892084E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0106493083622776E-15</c:v>
+                  <c:v>1.6667224529845286E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3766,10 +3766,10 @@
                   <c:v>0.74608213465529372</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48806516152707335</c:v>
+                  <c:v>0.40193601537524049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2263789868978307</c:v>
+                  <c:v>9.3828132727390851E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3837,10 +3837,10 @@
                   <c:v>0.12434702244254969</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1830244355726536</c:v>
+                  <c:v>0.1722582923036742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22637898689782668</c:v>
+                  <c:v>0.18765626545477837</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3908,10 +3908,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.36604887114530288</c:v>
+                  <c:v>0.40193601537523233</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67913696069348406</c:v>
+                  <c:v>0.65679692909171605</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4215,10 +4215,10 @@
                   <c:v>0.39228279302382935</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19632255332528095</c:v>
+                  <c:v>0.18477416783555881</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4973931219045618E-15</c:v>
+                  <c:v>5.3859969299998629E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4286,10 +4286,10 @@
                   <c:v>0.19614139651191034</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.8161276662640476E-2</c:v>
+                  <c:v>9.2387083917779403E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2486965609522809E-15</c:v>
+                  <c:v>2.6929984649999314E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4357,10 +4357,10 @@
                   <c:v>0.98070698255957256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68712893663847641</c:v>
+                  <c:v>0.50812896154777687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36577071553361129</c:v>
+                  <c:v>7.5801168021764495E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4428,10 +4428,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19632255332528095</c:v>
+                  <c:v>0.27716125175333162</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36577071553361129</c:v>
+                  <c:v>0.45480700813061392</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4499,10 +4499,10 @@
                   <c:v>0.39228279302383462</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78529021330110993</c:v>
+                  <c:v>0.78529021330110849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0973121466008273</c:v>
+                  <c:v>0.98541518428299235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4806,13 +4806,13 @@
                   <c:v>1.1461339603488307</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18689195024977348</c:v>
+                  <c:v>0.18689195024977612</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40555568865156938</c:v>
+                  <c:v>0.22067744109561618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57039994023884211</c:v>
+                  <c:v>1.0028417127154065E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4883,10 +4883,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.22067744109561618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.56454969546208489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4951,13 +4951,13 @@
                   <c:v>0.11752148612594081</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.672298756244337E-2</c:v>
+                  <c:v>4.6722987562444029E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10138892216289234</c:v>
+                  <c:v>5.5169360273904046E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14259998505971053</c:v>
+                  <c:v>2.5071042817885162E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5093,13 +5093,13 @@
                   <c:v>1.4551839553362556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3737839004995489</c:v>
+                  <c:v>0.37378390049955224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60833353297735548</c:v>
+                  <c:v>0.44135488219123237</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57039994023885021</c:v>
+                  <c:v>2.0056834254308129E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5167,10 +5167,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.22067744109561618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.56454969546208489</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5238,10 +5238,10 @@
                   <c:v>9.3445975124888059E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10138892216289377</c:v>
+                  <c:v>0.11033872054780809</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0661691751838064E-15</c:v>
+                  <c:v>5.0142085635770323E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5309,10 +5309,10 @@
                   <c:v>4.6722987562444029E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0694461081446887E-2</c:v>
+                  <c:v>5.5169360273904046E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5330845875919032E-15</c:v>
+                  <c:v>2.5071042817885162E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5380,10 +5380,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30416676648867413</c:v>
+                  <c:v>5.5169360273904046E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85559991035826521</c:v>
+                  <c:v>0.14113742386552122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5451,10 +5451,10 @@
                   <c:v>9.3445975124887226E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15208338324433887</c:v>
+                  <c:v>0.16550808082171017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14259998505971255</c:v>
+                  <c:v>0.14113742386552372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5519,13 +5519,13 @@
                   <c:v>1.1027890434022726E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3361493781221682E-3</c:v>
+                  <c:v>2.3361493781221187E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0694461081446174E-3</c:v>
+                  <c:v>2.7584680136951045E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1299992529855263E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5590,13 +5590,13 @@
                   <c:v>3.3061556548524024E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3361493781221602E-2</c:v>
+                  <c:v>2.3361493781220356E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6041691622169436E-2</c:v>
+                  <c:v>0.30343148150646637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14259998505971</c:v>
+                  <c:v>0.70568711932760853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5661,13 +5661,13 @@
                   <c:v>0.29149825225787274</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.7748331965543515E-2</c:v>
+                  <c:v>6.7748331965544334E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22305562875836379</c:v>
+                  <c:v>0.35584237376667383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42066995592614842</c:v>
+                  <c:v>0.70568711932760853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5990,13 +5990,13 @@
                   <c:v>3.5490739281993244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4405620659942902</c:v>
+                  <c:v>1.4405620659942966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4622018506887151</c:v>
+                  <c:v>0.98345331717623241</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3912193664362154</c:v>
+                  <c:v>3.6992079412221778E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6067,10 +6067,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.53823766120882</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.3769504767367924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6135,13 +6135,13 @@
                   <c:v>4.5301466613559409</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6031517889040692</c:v>
+                  <c:v>1.6031517889040712</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3009018369217915</c:v>
+                  <c:v>0.86072860700873022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96936383076661992</c:v>
+                  <c:v>8.9069178491856055E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6277,13 +6277,13 @@
                   <c:v>3.9173540691601554</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8478370768664552</c:v>
+                  <c:v>2.8478370768664614</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6165992822433761</c:v>
+                  <c:v>1.9717914287132665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8405760652730039</c:v>
+                  <c:v>0.23242347346733472</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6351,10 +6351,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.42437969441464651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.0856724912732401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6422,10 +6422,10 @@
                   <c:v>0.28316962159056985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30723915806937507</c:v>
+                  <c:v>0.33435975923578209</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5352027803587291E-14</c:v>
+                  <c:v>1.5194571404778885E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6493,10 +6493,10 @@
                   <c:v>0.33109382213482125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.758711753811392</c:v>
+                  <c:v>0.94424789719374114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95855016884281752</c:v>
+                  <c:v>1.1243283329890268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6564,10 +6564,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69128810565607757</c:v>
+                  <c:v>0.12538490971341829</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9445452508142391</c:v>
+                  <c:v>0.32076687242163915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6635,10 +6635,10 @@
                   <c:v>9.3445975124887226E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15208338324433887</c:v>
+                  <c:v>0.16550808082171017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14259998505971255</c:v>
+                  <c:v>0.14113742386552372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6703,13 +6703,13 @@
                   <c:v>0.11027890434022726</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3361493781221682E-2</c:v>
+                  <c:v>2.3361493781221186E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0694461081446172E-2</c:v>
+                  <c:v>2.7584680136951045E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1299992529855263E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6774,13 +6774,13 @@
                   <c:v>3.3061556548524024E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3361493781221602E-2</c:v>
+                  <c:v>2.3361493781220356E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6041691622169436E-2</c:v>
+                  <c:v>0.30343148150646637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14259998505971</c:v>
+                  <c:v>0.70568711932760853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6845,13 +6845,13 @@
                   <c:v>0.29149825225787274</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.7748331965543515E-2</c:v>
+                  <c:v>6.7748331965544334E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22305562875836379</c:v>
+                  <c:v>0.35584237376667383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42066995592614842</c:v>
+                  <c:v>0.70568711932760853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7163,10 +7163,10 @@
                   <c:v>107.30895803166814</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.717729703678472</c:v>
+                  <c:v>53.136431315310276</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.519737141436462</c:v>
+                  <c:v>4.252445526021706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7227,10 +7227,10 @@
                   <c:v>107.30895803166814</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.717729703678472</c:v>
+                  <c:v>53.136431315310276</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.519737141436462</c:v>
+                  <c:v>4.252445526021706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7520,10 +7520,10 @@
                   <c:v>75.006123937346317</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.645227069558828</c:v>
+                  <c:v>37.856630705271023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.699861164968839</c:v>
+                  <c:v>5.2637582460070709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12163,30 +12163,30 @@
         </row>
         <row r="32">
           <cell r="B32">
-            <v>1.9632255332527817</v>
+            <v>1.8477416783555618</v>
           </cell>
           <cell r="C32">
-            <v>1.2838357799983027</v>
+            <v>1.2083160282336982</v>
           </cell>
           <cell r="D32">
-            <v>1.2201629038176878</v>
+            <v>1.1483886153578253</v>
           </cell>
           <cell r="E32">
-            <v>0.90511001758406251</v>
+            <v>0.85186825184382464</v>
           </cell>
         </row>
         <row r="42">
           <cell r="B42">
-            <v>1.828853577668063</v>
+            <v>1.5160233604353761</v>
           </cell>
           <cell r="C42">
-            <v>1.0744853278380218</v>
+            <v>0.89069178491836509</v>
           </cell>
           <cell r="D42">
-            <v>1.1318949344891374</v>
+            <v>0.93828132727389524</v>
           </cell>
           <cell r="E42">
-            <v>0.7575170042188536</v>
+            <v>0.62794172718142149</v>
           </cell>
         </row>
       </sheetData>
@@ -12240,13 +12240,13 @@
             <v>5.0000000000000711E-2</v>
           </cell>
           <cell r="E32">
-            <v>0.35000000000000142</v>
+            <v>0.27499999999999858</v>
           </cell>
           <cell r="F32">
-            <v>0.10000000000000142</v>
+            <v>0.14999999999999858</v>
           </cell>
           <cell r="G32">
-            <v>0.39999999999999858</v>
+            <v>0.42499999999999716</v>
           </cell>
         </row>
         <row r="42">
@@ -12257,13 +12257,13 @@
             <v>1.7763568394002505E-15</v>
           </cell>
           <cell r="E42">
-            <v>0.19999999999999929</v>
+            <v>4.9999999999997158E-2</v>
           </cell>
           <cell r="F42">
-            <v>0.19999999999999929</v>
+            <v>0.30000000000000071</v>
           </cell>
           <cell r="G42">
-            <v>0.59999999999999432</v>
+            <v>0.64999999999999858</v>
           </cell>
         </row>
       </sheetData>
@@ -12307,16 +12307,16 @@
             <v>5.0000000000000711E-2</v>
           </cell>
           <cell r="D32">
-            <v>0.64999999999999858</v>
+            <v>0.45000000000000284</v>
           </cell>
           <cell r="E32">
             <v>0</v>
           </cell>
           <cell r="F32">
-            <v>0.10000000000000142</v>
+            <v>0.20000000000000284</v>
           </cell>
           <cell r="G32">
-            <v>0.19999999999999929</v>
+            <v>0.29999999999999716</v>
           </cell>
         </row>
         <row r="42">
@@ -12324,16 +12324,16 @@
             <v>1.7763568394002505E-15</v>
           </cell>
           <cell r="D42">
-            <v>0.49999999999999645</v>
+            <v>0.10000000000000853</v>
           </cell>
           <cell r="E42">
             <v>0</v>
           </cell>
           <cell r="F42">
-            <v>0.19999999999999929</v>
+            <v>0.39999999999999858</v>
           </cell>
           <cell r="G42">
-            <v>0.29999999999999716</v>
+            <v>0.49999999999999289</v>
           </cell>
         </row>
       </sheetData>
@@ -12380,13 +12380,13 @@
             <v>5.0000000000000711E-2</v>
           </cell>
           <cell r="E32">
-            <v>0.39999999999999858</v>
+            <v>0.35000000000000142</v>
           </cell>
           <cell r="F32">
             <v>0.15000000000000036</v>
           </cell>
           <cell r="G32">
-            <v>0.29999999999999716</v>
+            <v>0.34999999999999432</v>
           </cell>
         </row>
         <row r="42">
@@ -12397,13 +12397,13 @@
             <v>1.7763568394002505E-15</v>
           </cell>
           <cell r="E42">
-            <v>0.20000000000000284</v>
+            <v>0.10000000000000142</v>
           </cell>
           <cell r="F42">
             <v>0.19999999999999929</v>
           </cell>
           <cell r="G42">
-            <v>0.60000000000000142</v>
+            <v>0.69999999999998863</v>
           </cell>
         </row>
       </sheetData>
@@ -12450,13 +12450,13 @@
             <v>0</v>
           </cell>
           <cell r="E32">
-            <v>0.30000000000000071</v>
+            <v>0.25</v>
           </cell>
           <cell r="F32">
             <v>0.15000000000000036</v>
           </cell>
           <cell r="G32">
-            <v>0.44999999999999929</v>
+            <v>0.5</v>
           </cell>
         </row>
         <row r="42">
@@ -12467,13 +12467,13 @@
             <v>0</v>
           </cell>
           <cell r="E42">
-            <v>0.20000000000000284</v>
+            <v>9.9999999999997868E-2</v>
           </cell>
           <cell r="F42">
             <v>0.19999999999999929</v>
           </cell>
           <cell r="G42">
-            <v>0.60000000000000142</v>
+            <v>0.69999999999999574</v>
           </cell>
         </row>
       </sheetData>
@@ -12521,19 +12521,19 @@
         </row>
         <row r="22">
           <cell r="B22">
-            <v>0.2</v>
+            <v>0.20000000000000284</v>
           </cell>
           <cell r="C22">
             <v>0</v>
           </cell>
           <cell r="D22">
-            <v>0.05</v>
+            <v>5.0000000000000711E-2</v>
           </cell>
           <cell r="E22">
             <v>0</v>
           </cell>
           <cell r="F22">
-            <v>0.40000000000000213</v>
+            <v>0.40000000000000568</v>
           </cell>
           <cell r="G22">
             <v>0</v>
@@ -12551,33 +12551,33 @@
             <v>0.10000000000000053</v>
           </cell>
           <cell r="L22">
-            <v>2.5000000000000001E-3</v>
+            <v>2.4999999999999467E-3</v>
           </cell>
           <cell r="M22">
-            <v>2.4999999999999911E-2</v>
+            <v>2.4999999999998579E-2</v>
           </cell>
           <cell r="N22">
-            <v>7.2500000000000675E-2</v>
+            <v>7.2500000000001563E-2</v>
           </cell>
         </row>
         <row r="32">
           <cell r="B32">
-            <v>0.2</v>
+            <v>0.10000000000000142</v>
           </cell>
           <cell r="C32">
-            <v>0</v>
+            <v>0.10000000000000142</v>
           </cell>
           <cell r="D32">
-            <v>0.05</v>
+            <v>2.5000000000000355E-2</v>
           </cell>
           <cell r="E32">
             <v>0</v>
           </cell>
           <cell r="F32">
-            <v>0.30000000000000071</v>
+            <v>0.20000000000000284</v>
           </cell>
           <cell r="G32">
-            <v>0</v>
+            <v>0.10000000000000142</v>
           </cell>
           <cell r="H32">
             <v>5.0000000000000711E-2</v>
@@ -12586,39 +12586,39 @@
             <v>2.5000000000000355E-2</v>
           </cell>
           <cell r="J32">
-            <v>0.14999999999999858</v>
+            <v>2.5000000000000355E-2</v>
           </cell>
           <cell r="K32">
             <v>7.5000000000000178E-2</v>
           </cell>
           <cell r="L32">
-            <v>2.5000000000000001E-3</v>
+            <v>1.2499999999999734E-3</v>
           </cell>
           <cell r="M32">
-            <v>3.7500000000000089E-2</v>
+            <v>0.13749999999999929</v>
           </cell>
           <cell r="N32">
-            <v>0.11000000000000032</v>
+            <v>0.16124999999999901</v>
           </cell>
         </row>
         <row r="42">
           <cell r="B42">
-            <v>0.2</v>
+            <v>3.5527136788005009E-15</v>
           </cell>
           <cell r="C42">
-            <v>0</v>
+            <v>0.19999999999999929</v>
           </cell>
           <cell r="D42">
-            <v>0.05</v>
+            <v>8.8817841970012523E-16</v>
           </cell>
           <cell r="E42">
             <v>0</v>
           </cell>
           <cell r="F42">
-            <v>0.20000000000000284</v>
+            <v>7.1054273576010019E-15</v>
           </cell>
           <cell r="G42">
-            <v>0</v>
+            <v>0.19999999999999929</v>
           </cell>
           <cell r="H42">
             <v>1.7763568394002505E-15</v>
@@ -12627,19 +12627,19 @@
             <v>8.8817841970012523E-16</v>
           </cell>
           <cell r="J42">
-            <v>0.30000000000000071</v>
+            <v>4.9999999999999822E-2</v>
           </cell>
           <cell r="K42">
             <v>5.0000000000000711E-2</v>
           </cell>
           <cell r="L42">
-            <v>2.5000000000000001E-3</v>
+            <v>0</v>
           </cell>
           <cell r="M42">
-            <v>4.9999999999999822E-2</v>
+            <v>0.25</v>
           </cell>
           <cell r="N42">
-            <v>0.14750000000000085</v>
+            <v>0.25</v>
           </cell>
         </row>
       </sheetData>
@@ -13037,7 +13037,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -13104,7 +13104,7 @@
         <v>5</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -13121,7 +13121,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -13138,7 +13138,7 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -13155,7 +13155,7 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
@@ -13175,7 +13175,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -13238,13 +13238,13 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H3">
         <f>SUM(C3:G3)</f>
@@ -13286,16 +13286,16 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <f>SUM(C5:G5)</f>
@@ -13340,13 +13340,13 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>20</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <f>SUM(C7:G7)</f>
@@ -13391,13 +13391,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>20</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H9">
         <f>SUM(C9:G9)</f>
@@ -13418,7 +13418,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -13523,22 +13523,22 @@
         <v>2050</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>20</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -13547,19 +13547,19 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="K3">
         <v>5</v>
       </c>
       <c r="L3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="N3">
-        <v>14.75</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <f>SUM(B3:N3)</f>
@@ -13579,8 +13579,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -13680,23 +13680,23 @@
       </c>
       <c r="C4">
         <f>'[1]Consumption (EJyr)'!$B$32*[1]sIND!C32</f>
-        <v>0.19632255332528095</v>
+        <v>0.18477416783555881</v>
       </c>
       <c r="D4">
         <f>'[1]Consumption (EJyr)'!$B$32*[1]sIND!D32</f>
-        <v>9.8161276662640476E-2</v>
+        <v>9.2387083917779403E-2</v>
       </c>
       <c r="E4">
         <f>'[1]Consumption (EJyr)'!$B$32*[1]sIND!E32</f>
-        <v>0.68712893663847641</v>
+        <v>0.50812896154777687</v>
       </c>
       <c r="F4">
         <f>'[1]Consumption (EJyr)'!$B$32*[1]sIND!F32</f>
-        <v>0.19632255332528095</v>
+        <v>0.27716125175333162</v>
       </c>
       <c r="G4">
         <f>'[1]Consumption (EJyr)'!$B$32*[1]sIND!G32</f>
-        <v>0.78529021330110993</v>
+        <v>0.78529021330110849</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -13705,23 +13705,23 @@
       </c>
       <c r="C5">
         <f>'[1]Consumption (EJyr)'!$B$42*[1]sIND!C42</f>
-        <v>6.4973931219045618E-15</v>
+        <v>5.3859969299998629E-15</v>
       </c>
       <c r="D5">
         <f>'[1]Consumption (EJyr)'!$B$42*[1]sIND!D42</f>
-        <v>3.2486965609522809E-15</v>
+        <v>2.6929984649999314E-15</v>
       </c>
       <c r="E5">
         <f>'[1]Consumption (EJyr)'!$B$42*[1]sIND!E42</f>
-        <v>0.36577071553361129</v>
+        <v>7.5801168021764495E-2</v>
       </c>
       <c r="F5">
         <f>'[1]Consumption (EJyr)'!$B$42*[1]sIND!F42</f>
-        <v>0.36577071553361129</v>
+        <v>0.45480700813061392</v>
       </c>
       <c r="G5">
         <f>'[1]Consumption (EJyr)'!$B$42*[1]sIND!G42</f>
-        <v>1.0973121466008273</v>
+        <v>0.98541518428299235</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
@@ -13783,11 +13783,11 @@
       </c>
       <c r="C8">
         <f>'[1]Consumption (EJyr)'!$C$32*[1]sTRA!C32</f>
-        <v>6.4191788999916052E-2</v>
+        <v>6.0415801411685767E-2</v>
       </c>
       <c r="D8">
         <f>'[1]Consumption (EJyr)'!$C$32*[1]sTRA!D32</f>
-        <v>0.83449325699889487</v>
+        <v>0.54374221270516765</v>
       </c>
       <c r="E8">
         <f>'[1]Consumption (EJyr)'!$C$32*[1]sTRA!E32</f>
@@ -13795,11 +13795,11 @@
       </c>
       <c r="F8">
         <f>'[1]Consumption (EJyr)'!$C$32*[1]sTRA!F32</f>
-        <v>0.1283835779998321</v>
+        <v>0.24166320564674307</v>
       </c>
       <c r="G8">
         <f>'[1]Consumption (EJyr)'!$C$32*[1]sTRA!G32</f>
-        <v>0.2567671559996596</v>
+        <v>0.36249480847010601</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
@@ -13808,11 +13808,11 @@
       </c>
       <c r="C9">
         <f>'[1]Consumption (EJyr)'!$C$42*[1]sTRA!C42</f>
-        <v>1.9086693609402903E-15</v>
+        <v>1.5821864439373547E-15</v>
       </c>
       <c r="D9">
         <f>'[1]Consumption (EJyr)'!$C$42*[1]sTRA!D42</f>
-        <v>0.5372426639190071</v>
+        <v>8.9069178491844106E-2</v>
       </c>
       <c r="E9">
         <f>'[1]Consumption (EJyr)'!$C$42*[1]sTRA!E42</f>
@@ -13820,11 +13820,11 @@
       </c>
       <c r="F9">
         <f>'[1]Consumption (EJyr)'!$C$42*[1]sTRA!F42</f>
-        <v>0.21489706556760357</v>
+        <v>0.35627671396734478</v>
       </c>
       <c r="G9">
         <f>'[1]Consumption (EJyr)'!$C$42*[1]sTRA!G42</f>
-        <v>0.32234559835140347</v>
+        <v>0.44534589245917622</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -13886,23 +13886,23 @@
       </c>
       <c r="C12">
         <f>'[1]Consumption (EJyr)'!$D$32*[1]sCOM!C32</f>
-        <v>0.12201629038177052</v>
+        <v>0.11483886153578417</v>
       </c>
       <c r="D12">
         <f>'[1]Consumption (EJyr)'!$D$32*[1]sCOM!D32</f>
-        <v>6.1008145190885259E-2</v>
+        <v>5.7419430767892084E-2</v>
       </c>
       <c r="E12">
         <f>'[1]Consumption (EJyr)'!$D$32*[1]sCOM!E32</f>
-        <v>0.48806516152707335</v>
+        <v>0.40193601537524049</v>
       </c>
       <c r="F12">
         <f>'[1]Consumption (EJyr)'!$D$32*[1]sCOM!F32</f>
-        <v>0.1830244355726536</v>
+        <v>0.1722582923036742</v>
       </c>
       <c r="G12">
         <f>'[1]Consumption (EJyr)'!$D$32*[1]sCOM!G32</f>
-        <v>0.36604887114530288</v>
+        <v>0.40193601537523233</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
@@ -13911,23 +13911,23 @@
       </c>
       <c r="C13">
         <f>'[1]Consumption (EJyr)'!$D$42*[1]sCOM!C42</f>
-        <v>4.0212986167245552E-15</v>
+        <v>3.3334449059690571E-15</v>
       </c>
       <c r="D13">
         <f>'[1]Consumption (EJyr)'!$D$42*[1]sCOM!D42</f>
-        <v>2.0106493083622776E-15</v>
+        <v>1.6667224529845286E-15</v>
       </c>
       <c r="E13">
         <f>'[1]Consumption (EJyr)'!$D$42*[1]sCOM!E42</f>
-        <v>0.2263789868978307</v>
+        <v>9.3828132727390851E-2</v>
       </c>
       <c r="F13">
         <f>'[1]Consumption (EJyr)'!$D$42*[1]sCOM!F42</f>
-        <v>0.22637898689782668</v>
+        <v>0.18765626545477837</v>
       </c>
       <c r="G13">
         <f>'[1]Consumption (EJyr)'!$D$42*[1]sCOM!G42</f>
-        <v>0.67913696069348406</v>
+        <v>0.65679692909171605</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
@@ -13989,7 +13989,7 @@
       </c>
       <c r="C16">
         <f>'[1]Consumption (EJyr)'!$E$32*[1]sRES!C32</f>
-        <v>9.0511001758407539E-2</v>
+        <v>8.5186825184383669E-2</v>
       </c>
       <c r="D16">
         <f>'[1]Consumption (EJyr)'!$E$32*[1]sRES!D32</f>
@@ -13997,15 +13997,15 @@
       </c>
       <c r="E16">
         <f>'[1]Consumption (EJyr)'!$E$32*[1]sRES!E32</f>
-        <v>0.2715330052752194</v>
+        <v>0.21296706296095616</v>
       </c>
       <c r="F16">
         <f>'[1]Consumption (EJyr)'!$E$32*[1]sRES!F32</f>
-        <v>0.1357665026376097</v>
+        <v>0.12778023777657399</v>
       </c>
       <c r="G16">
         <f>'[1]Consumption (EJyr)'!$E$32*[1]sRES!G32</f>
-        <v>0.40729950791282749</v>
+        <v>0.42593412592191232</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.4">
@@ -14014,7 +14014,7 @@
       </c>
       <c r="C17">
         <f>'[1]Consumption (EJyr)'!$E$42*[1]sRES!C42</f>
-        <v>2.6912410228122979E-15</v>
+        <v>2.2308971636470485E-15</v>
       </c>
       <c r="D17">
         <f>'[1]Consumption (EJyr)'!$E$42*[1]sRES!D42</f>
@@ -14022,15 +14022,15 @@
       </c>
       <c r="E17">
         <f>'[1]Consumption (EJyr)'!$E$42*[1]sRES!E42</f>
-        <v>0.15150340084377287</v>
+        <v>6.2794172718140806E-2</v>
       </c>
       <c r="F17">
         <f>'[1]Consumption (EJyr)'!$E$42*[1]sRES!F42</f>
-        <v>0.15150340084377018</v>
+        <v>0.12558834543628386</v>
       </c>
       <c r="G17">
         <f>'[1]Consumption (EJyr)'!$E$42*[1]sRES!G42</f>
-        <v>0.45451020253131325</v>
+        <v>0.43955920902699236</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.4">
@@ -14092,23 +14092,23 @@
       </c>
       <c r="C20">
         <f>SUM(C4,C8,C12,C16)</f>
-        <v>0.47304163446537506</v>
+        <v>0.44521565596741242</v>
       </c>
       <c r="D20">
         <f t="shared" ref="D20:G20" si="2">SUM(D4,D8,D12,D16)</f>
-        <v>0.99366267885242066</v>
+        <v>0.69354872739083917</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>1.4467271034407692</v>
+        <v>1.1230320398839735</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>0.64349706953537633</v>
+        <v>0.81886298748032282</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>1.8154057483588999</v>
+        <v>1.975655163068359</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
@@ -14117,23 +14117,23 @@
       </c>
       <c r="C21">
         <f>SUM(C5,C9,C13,C17)</f>
-        <v>1.5118602122381706E-14</v>
+        <v>1.2532525443553324E-14</v>
       </c>
       <c r="D21">
         <f t="shared" ref="D21:G21" si="3">SUM(D5,D9,D13,D17)</f>
-        <v>0.53724266391901232</v>
+        <v>8.9069178491848464E-2</v>
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
-        <v>0.74365310327521483</v>
+        <v>0.23242347346729614</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>0.95855016884281175</v>
+        <v>1.124328332989021</v>
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>2.5533049081770285</v>
+        <v>2.5271172148608767</v>
       </c>
     </row>
   </sheetData>
@@ -14146,7 +14146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442FD7C5-04F0-4289-B7FC-E74A334AEBB6}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
@@ -14260,7 +14260,7 @@
       </c>
       <c r="B3">
         <f>[1]sELE!B22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
-        <v>0.18689195024977348</v>
+        <v>0.18689195024977612</v>
       </c>
       <c r="C3">
         <f>[1]sELE!C22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
@@ -14268,7 +14268,7 @@
       </c>
       <c r="D3">
         <f>[1]sELE!D22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
-        <v>4.672298756244337E-2</v>
+        <v>4.6722987562444029E-2</v>
       </c>
       <c r="E3">
         <f>[1]sELE!E22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
@@ -14276,7 +14276,7 @@
       </c>
       <c r="F3">
         <f>[1]sELE!F22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
-        <v>0.3737839004995489</v>
+        <v>0.37378390049955224</v>
       </c>
       <c r="G3">
         <f>[1]sELE!G22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
@@ -14300,15 +14300,15 @@
       </c>
       <c r="L3">
         <f>[1]sELE!L22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
-        <v>2.3361493781221682E-3</v>
+        <v>2.3361493781221187E-3</v>
       </c>
       <c r="M3">
         <f>[1]sELE!M22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
-        <v>2.3361493781221602E-2</v>
+        <v>2.3361493781220356E-2</v>
       </c>
       <c r="N3">
         <f>[1]sELE!N22*最終エネルギー消費!$G19/[1]LOSS!$B$12</f>
-        <v>6.7748331965543515E-2</v>
+        <v>6.7748331965544334E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
@@ -14317,15 +14317,15 @@
       </c>
       <c r="B4">
         <f>[1]sELE!B32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.40555568865156938</v>
+        <v>0.22067744109561618</v>
       </c>
       <c r="C4">
         <f>[1]sELE!C32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0</v>
+        <v>0.22067744109561618</v>
       </c>
       <c r="D4">
         <f>[1]sELE!D32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.10138892216289234</v>
+        <v>5.5169360273904046E-2</v>
       </c>
       <c r="E4">
         <f>[1]sELE!E32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
@@ -14333,39 +14333,39 @@
       </c>
       <c r="F4">
         <f>[1]sELE!F32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.60833353297735548</v>
+        <v>0.44135488219123237</v>
       </c>
       <c r="G4">
         <f>[1]sELE!G32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0</v>
+        <v>0.22067744109561618</v>
       </c>
       <c r="H4">
         <f>[1]sELE!H32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.10138892216289377</v>
+        <v>0.11033872054780809</v>
       </c>
       <c r="I4">
         <f>[1]sELE!I32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>5.0694461081446887E-2</v>
+        <v>5.5169360273904046E-2</v>
       </c>
       <c r="J4">
         <f>[1]sELE!J32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.30416676648867413</v>
+        <v>5.5169360273904046E-2</v>
       </c>
       <c r="K4">
         <f>[1]sELE!K32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.15208338324433887</v>
+        <v>0.16550808082171017</v>
       </c>
       <c r="L4">
         <f>[1]sELE!L32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>5.0694461081446174E-3</v>
+        <v>2.7584680136951045E-3</v>
       </c>
       <c r="M4">
         <f>[1]sELE!M32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>7.6041691622169436E-2</v>
+        <v>0.30343148150646637</v>
       </c>
       <c r="N4">
         <f>[1]sELE!N32*最終エネルギー消費!$G20/[1]LOSS!$B$12</f>
-        <v>0.22305562875836379</v>
+        <v>0.35584237376667383</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
@@ -14374,15 +14374,15 @@
       </c>
       <c r="B5">
         <f>[1]sELE!B42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.57039994023884211</v>
+        <v>1.0028417127154065E-14</v>
       </c>
       <c r="C5">
         <f>[1]sELE!C42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0</v>
+        <v>0.56454969546208489</v>
       </c>
       <c r="D5">
         <f>[1]sELE!D42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.14259998505971053</v>
+        <v>2.5071042817885162E-15</v>
       </c>
       <c r="E5">
         <f>[1]sELE!E42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
@@ -14390,39 +14390,39 @@
       </c>
       <c r="F5">
         <f>[1]sELE!F42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.57039994023885021</v>
+        <v>2.0056834254308129E-14</v>
       </c>
       <c r="G5">
         <f>[1]sELE!G42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0</v>
+        <v>0.56454969546208489</v>
       </c>
       <c r="H5">
         <f>[1]sELE!H42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>5.0661691751838064E-15</v>
+        <v>5.0142085635770323E-15</v>
       </c>
       <c r="I5">
         <f>[1]sELE!I42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>2.5330845875919032E-15</v>
+        <v>2.5071042817885162E-15</v>
       </c>
       <c r="J5">
         <f>[1]sELE!J42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.85559991035826521</v>
+        <v>0.14113742386552122</v>
       </c>
       <c r="K5">
         <f>[1]sELE!K42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.14259998505971255</v>
+        <v>0.14113742386552372</v>
       </c>
       <c r="L5">
         <f>[1]sELE!L42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>7.1299992529855263E-3</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f>[1]sELE!M42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.14259998505971</v>
+        <v>0.70568711932760853</v>
       </c>
       <c r="N5">
         <f>[1]sELE!N42*最終エネルギー消費!$G21/[1]LOSS!$B$12</f>
-        <v>0.42066995592614842</v>
+        <v>0.70568711932760853</v>
       </c>
     </row>
   </sheetData>
@@ -14555,7 +14555,7 @@
       </c>
       <c r="B3">
         <f>発電電力量!B3/[1]eELE!B$12+最終エネルギー消費!C19</f>
-        <v>1.4405620659942902</v>
+        <v>1.4405620659942966</v>
       </c>
       <c r="C3">
         <f>発電電力量!C3/[1]eELE!C$12</f>
@@ -14563,7 +14563,7 @@
       </c>
       <c r="D3">
         <f>発電電力量!D3/[1]eELE!D$12+最終エネルギー消費!D19</f>
-        <v>1.6031517889040692</v>
+        <v>1.6031517889040712</v>
       </c>
       <c r="E3">
         <f>発電電力量!E3/[1]eELE!E$12</f>
@@ -14571,7 +14571,7 @@
       </c>
       <c r="F3">
         <f>発電電力量!F3/[1]eELE!F$12+最終エネルギー消費!E19</f>
-        <v>2.8478370768664552</v>
+        <v>2.8478370768664614</v>
       </c>
       <c r="G3">
         <f>発電電力量!G3/[1]eELE!G$12</f>
@@ -14595,19 +14595,19 @@
       </c>
       <c r="L3">
         <f>発電電力量!L3/[1]eELE!L$12</f>
-        <v>2.3361493781221682E-2</v>
+        <v>2.3361493781221186E-2</v>
       </c>
       <c r="M3">
         <f>発電電力量!M3/[1]eELE!M$12</f>
-        <v>2.3361493781221602E-2</v>
+        <v>2.3361493781220356E-2</v>
       </c>
       <c r="N3">
         <f>発電電力量!N3/[1]eELE!N$12</f>
-        <v>6.7748331965543515E-2</v>
+        <v>6.7748331965544334E-2</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O5" si="0">SUM(B3:N3)</f>
-        <v>6.7137316701430816</v>
+        <v>6.7137316701430949</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
@@ -14616,15 +14616,15 @@
       </c>
       <c r="B4">
         <f>発電電力量!B4/[1]eELE!B$12+最終エネルギー消費!C20</f>
-        <v>1.4622018506887151</v>
+        <v>0.98345331717623241</v>
       </c>
       <c r="C4">
         <f>発電電力量!C4/[1]eELE!C$12</f>
-        <v>0</v>
+        <v>0.53823766120882</v>
       </c>
       <c r="D4">
         <f>発電電力量!D4/[1]eELE!D$12+最終エネルギー消費!D20</f>
-        <v>1.3009018369217915</v>
+        <v>0.86072860700873022</v>
       </c>
       <c r="E4">
         <f>発電電力量!E4/[1]eELE!E$12</f>
@@ -14632,43 +14632,43 @@
       </c>
       <c r="F4">
         <f>発電電力量!F4/[1]eELE!F$12+最終エネルギー消費!E20</f>
-        <v>2.6165992822433761</v>
+        <v>1.9717914287132665</v>
       </c>
       <c r="G4">
         <f>発電電力量!G4/[1]eELE!G$12</f>
-        <v>0</v>
+        <v>0.42437969441464651</v>
       </c>
       <c r="H4">
         <f>発電電力量!H4/[1]eELE!H$12</f>
-        <v>0.30723915806937507</v>
+        <v>0.33435975923578209</v>
       </c>
       <c r="I4">
         <f>発電電力量!I4/[1]eELE!I$12+最終エネルギー消費!F20</f>
-        <v>0.758711753811392</v>
+        <v>0.94424789719374114</v>
       </c>
       <c r="J4">
         <f>発電電力量!J4/[1]eELE!J$12</f>
-        <v>0.69128810565607757</v>
+        <v>0.12538490971341829</v>
       </c>
       <c r="K4">
         <f>発電電力量!K4/[1]eELE!K$12</f>
-        <v>0.15208338324433887</v>
+        <v>0.16550808082171017</v>
       </c>
       <c r="L4">
         <f>発電電力量!L4/[1]eELE!L$12</f>
-        <v>5.0694461081446172E-2</v>
+        <v>2.7584680136951045E-2</v>
       </c>
       <c r="M4">
         <f>発電電力量!M4/[1]eELE!M$12</f>
-        <v>7.6041691622169436E-2</v>
+        <v>0.30343148150646637</v>
       </c>
       <c r="N4">
         <f>発電電力量!N4/[1]eELE!N$12</f>
-        <v>0.22305562875836379</v>
+        <v>0.35584237376667383</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>7.6388171520970456</v>
+        <v>7.0349498908964385</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
@@ -14677,15 +14677,15 @@
       </c>
       <c r="B5">
         <f>発電電力量!B5/[1]eELE!B$12+最終エネルギー消費!C21</f>
-        <v>1.3912193664362154</v>
+        <v>3.6992079412221778E-14</v>
       </c>
       <c r="C5">
         <f>発電電力量!C5/[1]eELE!C$12</f>
-        <v>0</v>
+        <v>1.3769504767367924</v>
       </c>
       <c r="D5">
         <f>発電電力量!D5/[1]eELE!D$12+最終エネルギー消費!D21</f>
-        <v>0.96936383076661992</v>
+        <v>8.9069178491856055E-2</v>
       </c>
       <c r="E5">
         <f>発電電力量!E5/[1]eELE!E$12</f>
@@ -14693,43 +14693,43 @@
       </c>
       <c r="F5">
         <f>発電電力量!F5/[1]eELE!F$12+最終エネルギー消費!E21</f>
-        <v>1.8405760652730039</v>
+        <v>0.23242347346733472</v>
       </c>
       <c r="G5">
         <f>発電電力量!G5/[1]eELE!G$12</f>
-        <v>0</v>
+        <v>1.0856724912732401</v>
       </c>
       <c r="H5">
         <f>発電電力量!H5/[1]eELE!H$12</f>
-        <v>1.5352027803587291E-14</v>
+        <v>1.5194571404778885E-14</v>
       </c>
       <c r="I5">
         <f>発電電力量!I5/[1]eELE!I$12+最終エネルギー消費!F21</f>
-        <v>0.95855016884281752</v>
+        <v>1.1243283329890268</v>
       </c>
       <c r="J5">
         <f>発電電力量!J5/[1]eELE!J$12</f>
-        <v>1.9445452508142391</v>
+        <v>0.32076687242163915</v>
       </c>
       <c r="K5">
         <f>発電電力量!K5/[1]eELE!K$12</f>
-        <v>0.14259998505971255</v>
+        <v>0.14113742386552372</v>
       </c>
       <c r="L5">
         <f>発電電力量!L5/[1]eELE!L$12</f>
-        <v>7.1299992529855263E-2</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f>発電電力量!M5/[1]eELE!M$12</f>
-        <v>0.14259998505971</v>
+        <v>0.70568711932760853</v>
       </c>
       <c r="N5">
         <f>発電電力量!N5/[1]eELE!N$12</f>
-        <v>0.42066995592614842</v>
+        <v>0.70568711932760853</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>7.8814246007083373</v>
+        <v>5.7817224879006819</v>
       </c>
     </row>
   </sheetData>
@@ -14742,8 +14742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50135BD3-8D7E-4B8D-9FA6-DFD6C0FAE594}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="Y32" sqref="Y32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -14843,19 +14843,19 @@
       </c>
       <c r="C4">
         <f>最終エネルギー消費!C4*[1]EMF!$A$2</f>
-        <v>18.572113544571575</v>
+        <v>17.479636277243863</v>
       </c>
       <c r="E4">
         <f>最終エネルギー消費!D4*[1]EMF!$C$2</f>
-        <v>7.5976828136883734</v>
+        <v>7.1507602952361262</v>
       </c>
       <c r="G4">
         <f>最終エネルギー消費!E4*[1]EMF!$E$2</f>
-        <v>38.547933345418528</v>
+        <v>28.506034742830284</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>64.717729703678472</v>
+        <v>53.136431315310276</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
@@ -14864,19 +14864,19 @@
       </c>
       <c r="C5">
         <f>最終エネルギー消費!C5*[1]EMF!$A$2</f>
-        <v>6.1465338933217148E-13</v>
+        <v>5.0951530957798696E-13</v>
       </c>
       <c r="E5">
         <f>最終エネルギー消費!D5*[1]EMF!$C$2</f>
-        <v>2.5144911381770654E-13</v>
+        <v>2.0843808119099472E-13</v>
       </c>
       <c r="G5">
         <f>最終エネルギー消費!E5*[1]EMF!$E$2</f>
-        <v>20.519737141435595</v>
+        <v>4.2524455260209884</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>20.519737141436462</v>
+        <v>4.252445526021706</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
@@ -14930,11 +14930,11 @@
       </c>
       <c r="C8">
         <f>最終エネルギー消費!C8*[1]EMF!$A$2</f>
-        <v>6.0725432393920578</v>
+        <v>5.7153348135454731</v>
       </c>
       <c r="E8">
         <f>最終エネルギー消費!D8*[1]EMF!$C$2</f>
-        <v>64.589778091714464</v>
+        <v>42.085647263379983</v>
       </c>
       <c r="G8">
         <f>最終エネルギー消費!E8*[1]EMF!$E$2</f>
@@ -14942,7 +14942,7 @@
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>70.662321331106526</v>
+        <v>47.800982076925457</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.4">
@@ -14951,11 +14951,11 @@
       </c>
       <c r="C9">
         <f>最終エネルギー消費!C9*[1]EMF!$A$2</f>
-        <v>1.8056012154495146E-13</v>
+        <v>1.4967483759647375E-13</v>
       </c>
       <c r="E9">
         <f>最終エネルギー消費!D9*[1]EMF!$C$2</f>
-        <v>41.582582187331155</v>
+        <v>6.893954415268734</v>
       </c>
       <c r="G9">
         <f>最終エネルギー消費!E9*[1]EMF!$E$2</f>
@@ -14963,7 +14963,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>41.582582187331333</v>
+        <v>6.8939544152688841</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.4">
@@ -15017,19 +15017,19 @@
       </c>
       <c r="C12">
         <f>最終エネルギー消費!C12*[1]EMF!$A$2</f>
-        <v>11.54274107011549</v>
+        <v>10.863756301285182</v>
       </c>
       <c r="E12">
         <f>最終エネルギー消費!D12*[1]EMF!$C$2</f>
-        <v>4.722030437774519</v>
+        <v>4.4442639414348477</v>
       </c>
       <c r="G12">
         <f>最終エネルギー消費!E12*[1]EMF!$E$2</f>
-        <v>27.380455561668814</v>
+        <v>22.548610462550993</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
-        <v>43.645227069558828</v>
+        <v>37.856630705271023</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
@@ -15038,19 +15038,19 @@
       </c>
       <c r="C13">
         <f>最終エネルギー消費!C13*[1]EMF!$A$2</f>
-        <v>3.8041484914214289E-13</v>
+        <v>3.1534388810467278E-13</v>
       </c>
       <c r="E13">
         <f>最終エネルギー消費!D13*[1]EMF!$C$2</f>
-        <v>1.5562425646724031E-13</v>
+        <v>1.2900431786100253E-13</v>
       </c>
       <c r="G13">
         <f>最終エネルギー消費!E13*[1]EMF!$E$2</f>
-        <v>12.699861164968302</v>
+        <v>5.2637582460066268</v>
       </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>12.699861164968839</v>
+        <v>5.2637582460070709</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
@@ -15104,7 +15104,7 @@
       </c>
       <c r="C16">
         <f>最終エネルギー消費!C16*[1]EMF!$A$2</f>
-        <v>8.5623407663453523</v>
+        <v>8.0586736624426951</v>
       </c>
       <c r="E16">
         <f>最終エネルギー消費!D16*[1]EMF!$C$2</f>
@@ -15112,11 +15112,11 @@
       </c>
       <c r="G16">
         <f>最終エネルギー消費!E16*[1]EMF!$E$2</f>
-        <v>15.233001595939809</v>
+        <v>11.94745223210964</v>
       </c>
       <c r="P16">
         <f t="shared" si="0"/>
-        <v>23.795342362285162</v>
+        <v>20.006125894552333</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.4">
@@ -15125,7 +15125,7 @@
       </c>
       <c r="C17">
         <f>最終エネルギー消費!C17*[1]EMF!$A$2</f>
-        <v>2.5459140075804336E-13</v>
+        <v>2.1104287168101077E-13</v>
       </c>
       <c r="E17">
         <f>最終エネルギー消費!D17*[1]EMF!$C$2</f>
@@ -15133,11 +15133,11 @@
       </c>
       <c r="G17">
         <f>最終エネルギー消費!E17*[1]EMF!$E$2</f>
-        <v>8.4993407873356581</v>
+        <v>3.5227530894876993</v>
       </c>
       <c r="P17">
         <f t="shared" si="0"/>
-        <v>8.4993407873359121</v>
+        <v>3.5227530894879102</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.4">
@@ -15210,7 +15210,7 @@
       </c>
       <c r="C19">
         <f>発電電力量!B3/[1]eELE!B$12*[1]EMF!A$2</f>
-        <v>43.121898764947737</v>
+        <v>43.121898764948341</v>
       </c>
       <c r="D19">
         <f>発電電力量!C3/[1]eELE!C$12*[1]EMF!B$2</f>
@@ -15218,7 +15218,7 @@
       </c>
       <c r="E19">
         <f>発電電力量!D3/[1]eELE!D$12*[1]EMF!C$2</f>
-        <v>10.9586643555549</v>
+        <v>10.958664355555054</v>
       </c>
       <c r="F19">
         <f>発電電力量!E3/[1]eELE!E$12*[1]EMF!D$2</f>
@@ -15226,7 +15226,7 @@
       </c>
       <c r="G19">
         <f>発電電力量!F3/[1]eELE!F$12*[1]EMF!E$2</f>
-        <v>40.325532342355181</v>
+        <v>40.325532342355537</v>
       </c>
       <c r="H19">
         <f>発電電力量!G3/[1]eELE!G$12*[1]EMF!F$2</f>
@@ -15262,7 +15262,7 @@
       </c>
       <c r="P19">
         <f t="shared" si="0"/>
-        <v>94.40609546285782</v>
+        <v>94.406095462858929</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.4">
@@ -15271,15 +15271,15 @@
       </c>
       <c r="C20">
         <f>発電電力量!B4/[1]eELE!B$12*[1]EMF!A$2</f>
-        <v>93.574556454727968</v>
+        <v>50.917282750354367</v>
       </c>
       <c r="D20">
         <f>発電電力量!C4/[1]eELE!C$12*[1]EMF!B$2</f>
-        <v>0</v>
+        <v>2.5458641375177189</v>
       </c>
       <c r="E20">
         <f>発電電力量!D4/[1]eELE!D$12*[1]EMF!C$2</f>
-        <v>23.780310834569299</v>
+        <v>12.939722682424769</v>
       </c>
       <c r="F20">
         <f>発電電力量!E4/[1]eELE!E$12*[1]EMF!D$2</f>
@@ -15287,11 +15287,11 @@
       </c>
       <c r="G20">
         <f>発電電力量!F4/[1]eELE!F$12*[1]EMF!E$2</f>
-        <v>65.629829230826246</v>
+        <v>47.615401713323337</v>
       </c>
       <c r="H20">
         <f>発電電力量!G4/[1]eELE!G$12*[1]EMF!F$2</f>
-        <v>0</v>
+        <v>1.1903850428330836</v>
       </c>
       <c r="I20">
         <f>発電電力量!H4/[1]eELE!H$12*[1]EMF!G$2</f>
@@ -15303,7 +15303,7 @@
       </c>
       <c r="K20">
         <f>発電電力量!J4/[1]eELE!J$12*[1]EMF!I$2</f>
-        <v>-65.672370037327369</v>
+        <v>-11.911566422774737</v>
       </c>
       <c r="L20">
         <f>発電電力量!K4/[1]eELE!K$12*[1]EMF!J$2</f>
@@ -15323,7 +15323,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="0"/>
-        <v>117.31232648279615</v>
+        <v>103.29708990367854</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.4">
@@ -15332,15 +15332,15 @@
       </c>
       <c r="C21">
         <f>発電電力量!B5/[1]eELE!B$12*[1]EMF!A$2</f>
-        <v>131.60935206486454</v>
+        <v>2.3138738054360354E-12</v>
       </c>
       <c r="D21">
         <f>発電電力量!C5/[1]eELE!C$12*[1]EMF!B$2</f>
-        <v>0</v>
+        <v>6.5129757549650282</v>
       </c>
       <c r="E21">
         <f>発電電力量!D5/[1]eELE!D$12*[1]EMF!C$2</f>
-        <v>33.446178314004833</v>
+        <v>5.8802991336494286E-13</v>
       </c>
       <c r="F21">
         <f>発電電力量!E5/[1]eELE!E$12*[1]EMF!D$2</f>
@@ -15348,11 +15348,11 @@
       </c>
       <c r="G21">
         <f>発電電力量!F5/[1]eELE!F$12*[1]EMF!E$2</f>
-        <v>61.537378168075961</v>
+        <v>2.1638238493590115E-12</v>
       </c>
       <c r="H21">
         <f>発電電力量!G5/[1]eELE!G$12*[1]EMF!F$2</f>
-        <v>0</v>
+        <v>3.0453113380214387</v>
       </c>
       <c r="I21">
         <f>発電電力量!H5/[1]eELE!H$12*[1]EMF!G$2</f>
@@ -15364,7 +15364,7 @@
       </c>
       <c r="K21">
         <f>発電電力量!J5/[1]eELE!J$12*[1]EMF!I$2</f>
-        <v>-184.73179882735272</v>
+        <v>-30.472852880055719</v>
       </c>
       <c r="L21">
         <f>発電電力量!K5/[1]eELE!K$12*[1]EMF!J$2</f>
@@ -15384,7 +15384,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="0"/>
-        <v>41.861109719592633</v>
+        <v>-20.914565787064184</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.4">
@@ -15457,7 +15457,7 @@
       </c>
       <c r="C23">
         <f t="shared" ref="C23:P25" si="2">SUM(C3,C7,C11,C15,C19)</f>
-        <v>136.27717144305984</v>
+        <v>136.27717144306044</v>
       </c>
       <c r="D23">
         <f t="shared" si="2"/>
@@ -15465,7 +15465,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>124.083948461175</v>
+        <v>124.08394846117515</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
@@ -15473,7 +15473,7 @@
       </c>
       <c r="G23">
         <f t="shared" si="2"/>
-        <v>159.76366001220813</v>
+        <v>159.7636600122085</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
@@ -15509,7 +15509,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="2"/>
-        <v>420.12477991644295</v>
+        <v>420.12477991644403</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.4">
@@ -15518,15 +15518,15 @@
       </c>
       <c r="C24">
         <f t="shared" si="2"/>
-        <v>138.32429507515243</v>
+        <v>93.034683804871577</v>
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.5458641375177189</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>100.68980217774666</v>
+        <v>66.620394182475721</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
@@ -15534,11 +15534,11 @@
       </c>
       <c r="G24">
         <f t="shared" si="2"/>
-        <v>146.79121973385338</v>
+        <v>110.61749915081425</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1903850428330836</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
@@ -15550,7 +15550,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
-        <v>-65.672370037327369</v>
+        <v>-11.911566422774737</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
@@ -15570,7 +15570,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="2"/>
-        <v>320.13294694942516</v>
+        <v>262.09725989573758</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.4">
@@ -15579,15 +15579,15 @@
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
-        <v>131.60935206486596</v>
+        <v>3.49945071239618E-12</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5129757549650282</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>75.028760501336393</v>
+        <v>6.8939544152696595</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
@@ -15595,11 +15595,11 @@
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>103.25631726181551</v>
+        <v>13.038956861517478</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.0453113380214387</v>
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
@@ -15611,7 +15611,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
-        <v>-184.73179882735272</v>
+        <v>-30.472852880055719</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
@@ -15631,7 +15631,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="2"/>
-        <v>125.16263100066517</v>
+        <v>-0.98165451027861295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>